<commit_message>
Added more changes for tweet cleaner
</commit_message>
<xml_diff>
--- a/twitter/Tweet-Scale.xlsx
+++ b/twitter/Tweet-Scale.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="APPL" sheetId="4" r:id="rId2"/>
+    <sheet name="AAPL" sheetId="4" r:id="rId2"/>
     <sheet name="MSFT" sheetId="14" r:id="rId3"/>
     <sheet name="GE" sheetId="8" r:id="rId4"/>
     <sheet name="IBM" sheetId="9" r:id="rId5"/>
@@ -22,12 +22,12 @@
     <sheet name="MCD" sheetId="12" r:id="rId13"/>
     <sheet name="MMM" sheetId="13" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="364">
   <si>
     <t>AAPL</t>
   </si>
@@ -1110,9 +1110,6 @@
   </si>
   <si>
     <t>Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rating </t>
   </si>
   <si>
     <t>Irrevalent to IBM</t>
@@ -1753,7 +1750,7 @@
   <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3496,7 +3493,7 @@
         <v>44</v>
       </c>
       <c r="D124" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3507,7 +3504,7 @@
         <v>43021.694571759261</v>
       </c>
       <c r="C125" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -3538,7 +3535,7 @@
         <v>124</v>
       </c>
       <c r="D127" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3846,7 +3843,7 @@
         <v>37</v>
       </c>
       <c r="D149" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -4014,7 +4011,7 @@
         <v>141</v>
       </c>
       <c r="D161" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4097,7 +4094,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5493,7 +5490,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5527,7 +5524,7 @@
         <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5751,7 +5748,7 @@
         <v>303</v>
       </c>
       <c r="D18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5821,7 +5818,7 @@
         <v>313</v>
       </c>
       <c r="D23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5947,7 +5944,7 @@
         <v>340</v>
       </c>
       <c r="D32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5961,7 +5958,7 @@
         <v>341</v>
       </c>
       <c r="D33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -6441,7 +6438,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6461,7 +6458,7 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>